<commit_message>
Update: Adjustment File Storage Service: Import File
</commit_message>
<xml_diff>
--- a/storage/daily-log-template.xlsx
+++ b/storage/daily-log-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/unjustorono/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\daily-activity-service\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC58BC9-D194-9643-8F98-6BAF5249AC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC6128D-585E-4CEA-9CCD-83C3D1B1484F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{7564F57E-4F96-9448-94C9-8E683FA45256}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="14520" xr2:uid="{7564F57E-4F96-9448-94C9-8E683FA45256}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,18 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
     <t>What you've done today ?</t>
-  </si>
-  <si>
-    <t>Role</t>
   </si>
   <si>
     <t>Duration</t>
@@ -64,9 +56,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,19 +115,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,77 +462,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09112A9-AD59-014C-98D3-AFB801D43EFF}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="37" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="36">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
+      <c r="B1" s="13" t="s">
+        <v>4</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75">
       <c r="A2" s="2"/>
-      <c r="B2" s="6"/>
-      <c r="F2" s="10"/>
+      <c r="B2" s="5"/>
+      <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="15.75">
       <c r="A3" s="2"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" s="3" customFormat="1" ht="15.75">
       <c r="A4" s="2"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15.75">
       <c r="A5" s="1"/>
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>